<commit_message>
nma do subgrupo rato
</commit_message>
<xml_diff>
--- a/data/df_c.xlsx
+++ b/data/df_c.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PC LAB/DissAnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_70431CDD8F79A8D366075C52F37BD2720A49B649" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87DEB5B8-DB0B-4CB4-AB72-EA2A3053F504}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_B1471CDD8F79A8D366075C52F37BD272EA42F409" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8BA636D-4089-4C84-A664-576F5DF1A94B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="212">
   <si>
     <t>label</t>
   </si>
@@ -656,9 +656,6 @@
   </si>
   <si>
     <t>video analysis</t>
-  </si>
-  <si>
-    <t>257-259</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AR12" sqref="AR12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,7 +3531,7 @@
         <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
         <v>175</v>

</xml_diff>

<commit_message>
add analise de poder para uma possivel comparacao entre subgrupos
</commit_message>
<xml_diff>
--- a/data/df_c.xlsx
+++ b/data/df_c.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PC LAB/DissAnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_11571CDD8F79A8D366075C52F37BD272AA4E8235" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{459D8294-CFF4-4DEE-A249-A16F6671B60E}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_11571CDD8F79A8D366075C52F37BD272AA4E8235" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC6E57B2-0E4F-4B52-BD90-8292A5076220}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1047,8 +1047,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP7" sqref="AP7:AQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>